<commit_message>
re-ran optimization for w01_100.5
</commit_message>
<xml_diff>
--- a/results/optimization_results/cac/cac_results.xlsx
+++ b/results/optimization_results/cac/cac_results.xlsx
@@ -726,7 +726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,6 +999,236 @@
       </c>
       <c r="G11" t="n">
         <v>0.8969080230767617</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>628</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2.965601718751368</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>637</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8948364207292779</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.2265038621548684</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.09759263431911268</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="n">
+        <v>627</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.245351364593948</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.2582568596808386</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.272021389224577</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" t="n">
+        <v>638</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2.67683929251567</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3904905328228748</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="n">
+        <v>636</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.642464116218913</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9202976414121006</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.1868952056471511</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.97192326356339</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.5062142622216756</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" t="n">
+        <v>628</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.632362306672351</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.86579608944121</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>7</v>
+      </c>
+      <c r="B18" t="n">
+        <v>637</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.571086636207806</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.529333268663417</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2.014440803429157</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>8</v>
+      </c>
+      <c r="B19" t="n">
+        <v>628</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8441961990733206</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.848961237817112</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>9</v>
+      </c>
+      <c r="B20" t="n">
+        <v>627</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.4033350215703653</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.6328511528626054</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.3283095666231202</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.121984034631293</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.4355925982014164</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" t="n">
+        <v>643</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.049253329906997</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.1245359487357942</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.1583826196617993</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.174234501073174</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1984033032562611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>